<commit_message>
29/3 (incl. 26 - 28 march)
</commit_message>
<xml_diff>
--- a/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
+++ b/rivm_covid_19_data/rivm_covid_19_time_series/time_series_19-covid-Confirmed_province.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD13"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,26 @@
           <t>25-03-2020</t>
         </is>
       </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>26-03-2020</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>27-03-2020</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>28-03-2020</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>29-03-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -611,6 +631,18 @@
       <c r="AD2" t="n">
         <v>59</v>
       </c>
+      <c r="AE2" t="n">
+        <v>70</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>78</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>96</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>111</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -705,6 +737,18 @@
       <c r="AD3" t="n">
         <v>82</v>
       </c>
+      <c r="AE3" t="n">
+        <v>92</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>105</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>117</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -799,6 +843,18 @@
       <c r="AD4" t="n">
         <v>51</v>
       </c>
+      <c r="AE4" t="n">
+        <v>68</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>81</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>96</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>118</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -893,6 +949,18 @@
       <c r="AD5" t="n">
         <v>675</v>
       </c>
+      <c r="AE5" t="n">
+        <v>797</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>926</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>1058</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1235</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -987,6 +1055,18 @@
       <c r="AD6" t="n">
         <v>80</v>
       </c>
+      <c r="AE6" t="n">
+        <v>109</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>120</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>133</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1081,6 +1161,18 @@
       <c r="AD7" t="n">
         <v>765</v>
       </c>
+      <c r="AE7" t="n">
+        <v>858</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>943</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>1073</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>1168</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1175,6 +1267,18 @@
       <c r="AD8" t="n">
         <v>1861</v>
       </c>
+      <c r="AE8" t="n">
+        <v>2100</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>2426</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>2678</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>2950</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1269,6 +1373,18 @@
       <c r="AD9" t="n">
         <v>825</v>
       </c>
+      <c r="AE9" t="n">
+        <v>982</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>1175</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>1335</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>1484</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1363,6 +1479,18 @@
       <c r="AD10" t="n">
         <v>316</v>
       </c>
+      <c r="AE10" t="n">
+        <v>385</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>443</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>511</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>583</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1457,6 +1585,18 @@
       <c r="AD11" t="n">
         <v>547</v>
       </c>
+      <c r="AE11" t="n">
+        <v>628</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>716</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>797</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>880</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1551,6 +1691,18 @@
       <c r="AD12" t="n">
         <v>76</v>
       </c>
+      <c r="AE12" t="n">
+        <v>90</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>108</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>119</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1644,6 +1796,18 @@
       </c>
       <c r="AD13" t="n">
         <v>862</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>1015</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>1217</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>1470</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>1625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>